<commit_message>
Updated Use Case Doc
Updated Use Case Doc
</commit_message>
<xml_diff>
--- a/Diagrams_Documents/Use Case_Example.xlsx
+++ b/Diagrams_Documents/Use Case_Example.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8fa0bc907c9f8b7e/School/CIT 360/Code/Diagrams_Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ESD\OneDrive\School\CIT 360\Code\Diagrams_Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9E7507A-E494-4ED9-84CE-5CFFA223F204}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="49" documentId="8_{A9E7507A-E494-4ED9-84CE-5CFFA223F204}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{85C13CE9-8709-418B-A810-CE6148826C23}"/>
   <bookViews>
-    <workbookView xWindow="31875" yWindow="1440" windowWidth="21600" windowHeight="15345" xr2:uid="{C60C96B5-5365-40BB-A64C-4BFEEA64501B}"/>
+    <workbookView xWindow="31005" yWindow="1830" windowWidth="21600" windowHeight="15345" xr2:uid="{C60C96B5-5365-40BB-A64C-4BFEEA64501B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
-  <si>
-    <t>Use Case:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Summary:</t>
   </si>
@@ -63,38 +60,70 @@
     <t>Author:</t>
   </si>
   <si>
-    <t>Date:</t>
-  </si>
-  <si>
     <t>Bryce Blauser</t>
   </si>
   <si>
     <t>GuessNumber</t>
   </si>
   <si>
-    <t>Documents how the Number class functions</t>
-  </si>
-  <si>
     <t>The user selects the option to play Guess Number by pressing "N" from the main menu</t>
   </si>
   <si>
     <t>The user was able to successfully enter the main menu screen by entering a valid user name</t>
   </si>
   <si>
-    <t>No other success routes.  An error will be thrown if an invalid value is entered.</t>
-  </si>
-  <si>
-    <t>1. The system generates a random number between 1 and 10
-2. The user enters a valid number value into the guess prompt (between 1 and 10)</t>
-  </si>
-  <si>
-    <t>1. The system responds by notifying the user if they guessed the number correctly</t>
-  </si>
-  <si>
     <t>1. The guessed value must be a numeric between 1 and 10</t>
   </si>
   <si>
     <t>User can exit the prompts back to the main menu by entering "Q"</t>
+  </si>
+  <si>
+    <t>Use Case ID</t>
+  </si>
+  <si>
+    <t>Use Case Name:</t>
+  </si>
+  <si>
+    <t>Process Owner:</t>
+  </si>
+  <si>
+    <t>Creation Date:</t>
+  </si>
+  <si>
+    <t>Updated By:</t>
+  </si>
+  <si>
+    <t>Updated Date:</t>
+  </si>
+  <si>
+    <t>Documents how the Number class functions.  The number class should select a random number between 1 and 10, then compare it to the user input.</t>
+  </si>
+  <si>
+    <t>Performance Goal:</t>
+  </si>
+  <si>
+    <t>System should return the guess results in less than 1 second</t>
+  </si>
+  <si>
+    <t>1. User is able to enter the guess menu
+2. The system generates a random number between 1 and 10
+3. The user is able to enter a valid number value into the guess prompt (between 1 and 10)
+4. The system returns a response stating they guessed the number correctly</t>
+  </si>
+  <si>
+    <t>1. If the user does not guess the correct number ...
+2. The system will display the user's guess, and also the correct value
+3. The user will be given another opportunity to try again</t>
+  </si>
+  <si>
+    <t>1. The system responds by notifying the user if they guessed the number correctly
+2. The system will allow the user to play again, or exit to the main menu</t>
+  </si>
+  <si>
+    <t>Assumptions:</t>
+  </si>
+  <si>
+    <t>User is able to access the program via console.  No other connections methods exist</t>
   </si>
 </sst>
 </file>
@@ -159,7 +188,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -175,6 +204,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -490,104 +522,152 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4DFB2C8-1613-4212-BA71-7F2BB7F3AF73}">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="67.42578125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>12</v>
+        <v>15</v>
+      </c>
+      <c r="B1" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>5</v>
+        <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="79.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" s="5" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="B15" s="4">
+        <v>43637</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="B16" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="4">
-        <v>43637</v>
+      <c r="B17" s="4">
+        <v>43641</v>
       </c>
     </row>
   </sheetData>

</xml_diff>